<commit_message>
fixing one ID Lattes
</commit_message>
<xml_diff>
--- a/pq-1d-5years.xlsx
+++ b/pq-1d-5years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/perfil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BDE1AA-6135-1640-88AF-27007A79BCB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB85535E-BD38-1443-8BD5-D04915149DFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="27580" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,9 +622,6 @@
     <t>Anderson de Rezende Rocha</t>
   </si>
   <si>
-    <t>4251936710939360</t>
-  </si>
-  <si>
     <t>1130012055294645</t>
   </si>
   <si>
@@ -698,6 +695,9 @@
   </si>
   <si>
     <t>DI_Wyj0AAAAJ</t>
+  </si>
+  <si>
+    <t>1521815731111261</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1422,10 +1422,10 @@
         <v>199</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.2">
@@ -1433,10 +1433,10 @@
         <v>186</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.2">
@@ -2934,10 +2934,10 @@
         <v>187</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.2">
@@ -4269,10 +4269,10 @@
         <v>188</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.2">
@@ -4578,10 +4578,10 @@
         <v>189</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.2">
@@ -4592,7 +4592,7 @@
         <v>118</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29">
         <v>1994</v>
@@ -4723,10 +4723,10 @@
         <v>190</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.2">
@@ -5760,10 +5760,10 @@
         <v>191</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.2">
@@ -6516,7 +6516,7 @@
         <v>192</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>144</v>
@@ -7404,10 +7404,10 @@
         <v>193</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.2">
@@ -7415,10 +7415,10 @@
         <v>194</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.2">
@@ -7426,7 +7426,7 @@
         <v>195</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -7882,7 +7882,7 @@
         <v>196</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -7891,10 +7891,10 @@
         <v>197</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.2">
@@ -8332,10 +8332,10 @@
         <v>198</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>